<commit_message>
tix-8 fixed log error
</commit_message>
<xml_diff>
--- a/data/Routing.xlsx
+++ b/data/Routing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Computer Science Lessons\BankManagementSystem using Excel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073AA3D0-D45B-4D85-B188-9FC76F6DEA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DF9BA7-087B-418C-80B6-8D3C5C482FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7620" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7620" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -78,51 +78,21 @@
     <t>2021/09/30</t>
   </si>
   <si>
-    <t>17:29:53</t>
-  </si>
-  <si>
     <t>Checkings</t>
   </si>
   <si>
-    <t>Apple</t>
-  </si>
-  <si>
     <t>17:30:01</t>
   </si>
   <si>
     <t>Samsung</t>
   </si>
   <si>
-    <t>17:30:12</t>
-  </si>
-  <si>
-    <t>foodforless</t>
-  </si>
-  <si>
-    <t>17:30:19</t>
-  </si>
-  <si>
-    <t>Gas Station</t>
-  </si>
-  <si>
-    <t>17:30:33</t>
-  </si>
-  <si>
-    <t>Starbucks</t>
-  </si>
-  <si>
     <t>17:30:43</t>
   </si>
   <si>
     <t>chipotle</t>
   </si>
   <si>
-    <t>17:30:58</t>
-  </si>
-  <si>
-    <t>Inventory</t>
-  </si>
-  <si>
     <t>17:32:05</t>
   </si>
   <si>
@@ -163,6 +133,12 @@
   </si>
   <si>
     <t>16:02:21</t>
+  </si>
+  <si>
+    <t>16:32:37</t>
+  </si>
+  <si>
+    <t>test123</t>
   </si>
 </sst>
 </file>
@@ -507,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -586,16 +562,16 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="n">
-        <v>50000.0</v>
+      <c r="I2">
+        <v>50000</v>
       </c>
       <c r="J2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K2" s="5">
         <f>SUM(N2:P2)</f>
@@ -639,195 +615,215 @@
         <v>123000456</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="n">
-        <v>123.0</v>
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>123</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
       </c>
-      <c r="I6" t="n">
-        <v>123.0</v>
+      <c r="I6">
+        <v>123</v>
       </c>
       <c r="J6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
       </c>
-      <c r="I7" t="n">
-        <v>123.0</v>
+      <c r="I7">
+        <v>123</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="n">
-        <v>222.0</v>
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>222</v>
       </c>
       <c r="J8" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" t="n">
-        <v>-222.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>25</v>
+      </c>
+      <c r="K8">
+        <v>-222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
       </c>
-      <c r="I9" t="n">
-        <v>123.0</v>
+      <c r="I9">
+        <v>123</v>
       </c>
       <c r="J9" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" t="n">
-        <v>-123.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" t="n">
-        <v>123.0</v>
+        <v>16</v>
+      </c>
+      <c r="I10">
+        <v>123</v>
       </c>
       <c r="J10" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" t="n">
-        <v>-123.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>25</v>
+      </c>
+      <c r="K10">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" t="n">
-        <v>123.0</v>
+        <v>16</v>
+      </c>
+      <c r="I11">
+        <v>123</v>
       </c>
       <c r="J11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" t="n">
-        <v>-123.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
         <v>12</v>
       </c>
-      <c r="I12" t="n">
-        <v>123.0</v>
+      <c r="I12">
+        <v>123</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" t="n">
-        <v>-123.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
         <v>33</v>
-      </c>
-      <c r="G13" t="s">
-        <v>43</v>
       </c>
       <c r="H13" t="s">
         <v>11</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13">
+        <v>123</v>
+      </c>
+      <c r="J13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14">
+        <v>123</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="n">
         <v>123.0</v>
       </c>
-      <c r="J13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" t="n">
-        <v>-123.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" t="n">
-        <v>123.0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" t="n">
-        <v>-123.0</v>
+      <c r="J15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1376.0</v>
       </c>
     </row>
   </sheetData>
@@ -837,7 +833,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE80214-2342-4F0E-B6E2-2B95AADA1513}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
@@ -911,117 +907,136 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="n">
-        <v>8.0</v>
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
       </c>
       <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="4">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>123</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="4">
-        <f>Home!N2</f>
-        <v>1499</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4">
+        <v>222</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>-222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>123</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6">
+        <v>123</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>123</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="n">
         <v>123.0</v>
       </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="n">
-        <v>222.0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-222.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="n">
-        <v>123.0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-123.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="n">
-        <v>123.0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" t="n">
-        <v>-123.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="n">
-        <v>123.0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" t="n">
-        <v>-123.0</v>
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1376.0</v>
       </c>
     </row>
   </sheetData>
@@ -1105,57 +1120,56 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="n">
-        <v>200.0</v>
+      <c r="I2">
+        <v>200</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N2" s="4">
-        <f>Home!O2</f>
         <v>27300</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="n">
-        <v>123.0</v>
+      <c r="I3">
+        <v>123</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
         <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
       </c>
-      <c r="I4" t="n">
-        <v>123.0</v>
+      <c r="I4">
+        <v>123</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-123.0</v>
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>-123</v>
       </c>
     </row>
   </sheetData>
@@ -1167,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B09C839D-D397-4547-898D-3BD232822816}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1240,77 +1254,76 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="n">
-        <v>50000.0</v>
+      <c r="I2">
+        <v>50000</v>
       </c>
       <c r="J2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="N2" s="4">
-        <f>Home!P2</f>
         <v>315000111</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" t="n">
-        <v>123.0</v>
+      <c r="I3">
+        <v>123</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="n">
-        <v>123.0</v>
+      <c r="I4">
+        <v>123</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-123.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>-123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" t="n">
-        <v>123.0</v>
+      <c r="I5">
+        <v>123</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-123.0</v>
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>-123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tix-6 added read balance method
</commit_message>
<xml_diff>
--- a/data/Routing.xlsx
+++ b/data/Routing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Computer Science Lessons\BankManagementSystem using Excel\data\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>19:00:21</t>
+  </si>
+  <si>
+    <t>20:05:14</t>
+  </si>
+  <si>
+    <t>rich peoiple store</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
@@ -471,11 +477,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="1.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="1.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="16" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="1.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="1.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="14" max="16" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -622,6 +628,26 @@
     <row r="27" ht="15" x14ac:dyDescent="0.25"/>
     <row r="28" ht="15" x14ac:dyDescent="0.25"/>
     <row r="29" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="30">
+      <c r="F30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" t="n">
+        <v>9999.0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>31</v>
+      </c>
+      <c r="K30" t="n">
+        <v>89978.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -629,7 +655,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE80214-2342-4F0E-B6E2-2B95AADA1513}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
@@ -637,10 +663,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="1.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="1.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" style="1" width="1.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="1.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -768,6 +794,26 @@
       </c>
       <c r="K15">
         <v>99977.2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="n">
+        <v>9999.0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" t="n">
+        <v>89978.2</v>
       </c>
     </row>
   </sheetData>
@@ -785,10 +831,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="1.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="1.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" style="1" width="1.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="1.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -906,10 +952,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="1.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="1.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" style="1" width="1.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="1.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1030,7 +1076,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1043,9 +1089,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>99977.2</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>89978.2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>